<commit_message>
keine ahung was das ist, commit gibts trotzdem
</commit_message>
<xml_diff>
--- a/GVI & WUB/LS2/Stundensatzkalkulation_Vorlagen_LF2.8.xlsx
+++ b/GVI & WUB/LS2/Stundensatzkalkulation_Vorlagen_LF2.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/repos/Danger_Gang_GVI/GVI &amp; WUB/LS2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37642CFE-FE04-094F-92CF-51308C26E625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC11C68-D905-9D44-9836-3942E26DADD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="908" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" tabRatio="908" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SB S. 247_248" sheetId="38" r:id="rId1"/>
@@ -716,18 +716,6 @@
     <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -739,7 +727,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2473,11 +2473,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
@@ -2613,11 +2613,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
@@ -2815,7 +2815,7 @@
   </sheetPr>
   <dimension ref="D8:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -2830,600 +2830,600 @@
   </cols>
   <sheetData>
     <row r="8" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="56" t="s">
+      <c r="E8" s="64"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="56" t="s">
+      <c r="I8" s="64"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="67"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="66"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61" t="s">
+      <c r="G9" s="56"/>
+      <c r="H9" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="62" t="s">
+      <c r="I9" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="63" t="s">
+      <c r="J9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="61" t="s">
+      <c r="K9" s="56"/>
+      <c r="L9" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="62" t="s">
+      <c r="M9" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="63" t="s">
+      <c r="N9" s="59" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66">
+      <c r="E10" s="61"/>
+      <c r="F10" s="62">
         <v>300</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="64" t="s">
+      <c r="G10" s="56"/>
+      <c r="H10" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="66">
+      <c r="I10" s="61"/>
+      <c r="J10" s="62">
         <v>680</v>
       </c>
-      <c r="K10" s="60"/>
-      <c r="L10" s="64" t="s">
+      <c r="K10" s="56"/>
+      <c r="L10" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="65"/>
-      <c r="N10" s="66">
+      <c r="M10" s="61"/>
+      <c r="N10" s="62">
         <v>1400</v>
       </c>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="61">
         <v>20</v>
       </c>
-      <c r="F11" s="66">
+      <c r="F11" s="62">
         <f>F10/100*E11</f>
         <v>60</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="64" t="s">
+      <c r="G11" s="56"/>
+      <c r="H11" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="65">
+      <c r="I11" s="61">
         <v>20</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="62">
         <f>J10/100*I11</f>
         <v>136</v>
       </c>
-      <c r="K11" s="60"/>
-      <c r="L11" s="64" t="s">
+      <c r="K11" s="56"/>
+      <c r="L11" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="65">
+      <c r="M11" s="61">
         <v>15</v>
       </c>
-      <c r="N11" s="66">
+      <c r="N11" s="62">
         <f>N10/100*M11</f>
         <v>210</v>
       </c>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66">
+      <c r="E12" s="61"/>
+      <c r="F12" s="62">
         <f>F10-F11</f>
         <v>240</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="64" t="s">
+      <c r="G12" s="56"/>
+      <c r="H12" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="65"/>
-      <c r="J12" s="66">
+      <c r="I12" s="61"/>
+      <c r="J12" s="62">
         <f>J10-J11</f>
         <v>544</v>
       </c>
-      <c r="K12" s="60"/>
-      <c r="L12" s="64" t="s">
+      <c r="K12" s="56"/>
+      <c r="L12" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="65"/>
-      <c r="N12" s="66">
+      <c r="M12" s="61"/>
+      <c r="N12" s="62">
         <f>N10-N11</f>
         <v>1190</v>
       </c>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="61">
         <v>3</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="62">
         <f>F12/100*E13</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="64" t="s">
+      <c r="G13" s="56"/>
+      <c r="H13" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="65">
+      <c r="I13" s="61">
         <v>2</v>
       </c>
-      <c r="J13" s="66">
+      <c r="J13" s="62">
         <f>J12/100*I13</f>
         <v>10.88</v>
       </c>
-      <c r="K13" s="60"/>
-      <c r="L13" s="64" t="s">
+      <c r="K13" s="56"/>
+      <c r="L13" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="65">
+      <c r="M13" s="61">
         <v>2</v>
       </c>
-      <c r="N13" s="66">
+      <c r="N13" s="62">
         <f>N12/100*M13</f>
         <v>23.8</v>
       </c>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66">
+      <c r="E14" s="61"/>
+      <c r="F14" s="62">
         <f>F12-F13</f>
         <v>232.8</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="64" t="s">
+      <c r="G14" s="56"/>
+      <c r="H14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="66">
+      <c r="I14" s="61"/>
+      <c r="J14" s="62">
         <f>J12-J13</f>
         <v>533.12</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="64" t="s">
+      <c r="K14" s="56"/>
+      <c r="L14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="65"/>
-      <c r="N14" s="66">
+      <c r="M14" s="61"/>
+      <c r="N14" s="62">
         <f>N12-N13</f>
         <v>1166.2</v>
       </c>
     </row>
     <row r="15" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="61">
         <v>3</v>
       </c>
-      <c r="F15" s="66">
+      <c r="F15" s="62">
         <f>F14/100*E15</f>
         <v>6.9840000000000009</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="64" t="s">
+      <c r="G15" s="56"/>
+      <c r="H15" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="65">
+      <c r="I15" s="61">
         <v>7</v>
       </c>
-      <c r="J15" s="66">
+      <c r="J15" s="62">
         <f>J14/100*I15</f>
         <v>37.318399999999997</v>
       </c>
-      <c r="K15" s="60"/>
-      <c r="L15" s="64" t="s">
+      <c r="K15" s="56"/>
+      <c r="L15" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="65">
+      <c r="M15" s="61">
         <v>5</v>
       </c>
-      <c r="N15" s="66">
+      <c r="N15" s="62">
         <f>N14/100*M15</f>
         <v>58.31</v>
       </c>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66">
+      <c r="E16" s="61"/>
+      <c r="F16" s="62">
         <f>F14+F15</f>
         <v>239.78400000000002</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="64" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="65"/>
-      <c r="J16" s="66">
+      <c r="I16" s="61"/>
+      <c r="J16" s="62">
         <f>J14+J15</f>
         <v>570.4384</v>
       </c>
-      <c r="K16" s="60"/>
-      <c r="L16" s="64" t="s">
+      <c r="K16" s="56"/>
+      <c r="L16" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="65"/>
-      <c r="N16" s="66">
+      <c r="M16" s="61"/>
+      <c r="N16" s="62">
         <f>N14+N15</f>
         <v>1224.51</v>
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="61">
         <v>70</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F17" s="62">
         <f>F16/100*E17</f>
         <v>167.84880000000004</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="64" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="65">
+      <c r="I17" s="61">
         <v>75</v>
       </c>
-      <c r="J17" s="66">
+      <c r="J17" s="62">
         <f>J16/100*I17</f>
         <v>427.8288</v>
       </c>
-      <c r="K17" s="60"/>
-      <c r="L17" s="64" t="s">
+      <c r="K17" s="56"/>
+      <c r="L17" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="65">
+      <c r="M17" s="61">
         <v>70</v>
       </c>
-      <c r="N17" s="66">
+      <c r="N17" s="62">
         <f>N16/100*M17</f>
         <v>857.15700000000004</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D18" s="64" t="s">
+      <c r="D18" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66">
+      <c r="E18" s="61"/>
+      <c r="F18" s="62">
         <f>F16+F17</f>
         <v>407.63280000000009</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="64" t="s">
+      <c r="G18" s="56"/>
+      <c r="H18" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="66">
+      <c r="I18" s="61"/>
+      <c r="J18" s="62">
         <f>J16+J17</f>
         <v>998.2672</v>
       </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="64" t="s">
+      <c r="K18" s="56"/>
+      <c r="L18" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="65"/>
-      <c r="N18" s="66">
+      <c r="M18" s="61"/>
+      <c r="N18" s="62">
         <f>N16+N17</f>
         <v>2081.6669999999999</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="61">
         <v>8</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="62">
         <f>F18/100*E19</f>
         <v>32.610624000000008</v>
       </c>
-      <c r="G19" s="60"/>
-      <c r="H19" s="64" t="s">
+      <c r="G19" s="56"/>
+      <c r="H19" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="65">
+      <c r="I19" s="61">
         <v>10</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="62">
         <f>J18/100*I19</f>
         <v>99.826720000000009</v>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="64" t="s">
+      <c r="K19" s="56"/>
+      <c r="L19" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="65">
+      <c r="M19" s="61">
         <v>9</v>
       </c>
-      <c r="N19" s="66">
+      <c r="N19" s="62">
         <f>N18/100*M19</f>
         <v>187.35002999999998</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66">
+      <c r="E20" s="61"/>
+      <c r="F20" s="62">
         <f>F18+F19</f>
         <v>440.24342400000012</v>
       </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="64" t="s">
+      <c r="G20" s="56"/>
+      <c r="H20" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="65"/>
-      <c r="J20" s="66">
+      <c r="I20" s="61"/>
+      <c r="J20" s="62">
         <f>J18+J19</f>
         <v>1098.09392</v>
       </c>
-      <c r="K20" s="60"/>
-      <c r="L20" s="64" t="s">
+      <c r="K20" s="56"/>
+      <c r="L20" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="M20" s="65"/>
-      <c r="N20" s="66">
+      <c r="M20" s="61"/>
+      <c r="N20" s="62">
         <f>N18+N19</f>
         <v>2269.01703</v>
       </c>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66">
+      <c r="E21" s="61"/>
+      <c r="F21" s="62">
         <f>F20/(100-E21)*100-F20</f>
         <v>0</v>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="64" t="s">
+      <c r="G21" s="56"/>
+      <c r="H21" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="65">
+      <c r="I21" s="61">
         <v>3</v>
       </c>
-      <c r="J21" s="66">
+      <c r="J21" s="62">
         <f>J20/(100-I21)*100-J20</f>
         <v>33.961667628866053</v>
       </c>
-      <c r="K21" s="60"/>
-      <c r="L21" s="64" t="s">
+      <c r="K21" s="56"/>
+      <c r="L21" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="65">
+      <c r="M21" s="61">
         <v>3</v>
       </c>
-      <c r="N21" s="66">
+      <c r="N21" s="62">
         <f>N20/(100-M21)*100-N20</f>
         <v>70.175784432989531</v>
       </c>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66">
+      <c r="E22" s="61"/>
+      <c r="F22" s="62">
         <f>F20/100*E22</f>
         <v>0</v>
       </c>
-      <c r="G22" s="60"/>
-      <c r="H22" s="64" t="s">
+      <c r="G22" s="56"/>
+      <c r="H22" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="65">
+      <c r="I22" s="61">
         <v>0</v>
       </c>
-      <c r="J22" s="66">
+      <c r="J22" s="62">
         <f>J20/100*I22</f>
         <v>0</v>
       </c>
-      <c r="K22" s="60"/>
-      <c r="L22" s="64" t="s">
+      <c r="K22" s="56"/>
+      <c r="L22" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="65">
+      <c r="M22" s="61">
         <v>6</v>
       </c>
-      <c r="N22" s="66">
+      <c r="N22" s="62">
         <f>N20/100*M22</f>
         <v>136.14102179999998</v>
       </c>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D23" s="64" t="s">
+      <c r="D23" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="66">
+      <c r="E23" s="61"/>
+      <c r="F23" s="62">
         <f>F20+F21+F22</f>
         <v>440.24342400000012</v>
       </c>
-      <c r="G23" s="60"/>
-      <c r="H23" s="64" t="s">
+      <c r="G23" s="56"/>
+      <c r="H23" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="65"/>
-      <c r="J23" s="66">
+      <c r="I23" s="61"/>
+      <c r="J23" s="62">
         <f>J20+J21+J22</f>
         <v>1132.0555876288661</v>
       </c>
-      <c r="K23" s="60"/>
-      <c r="L23" s="64" t="s">
+      <c r="K23" s="56"/>
+      <c r="L23" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="65"/>
-      <c r="N23" s="66">
+      <c r="M23" s="61"/>
+      <c r="N23" s="62">
         <f>N20+N21+N22</f>
         <v>2475.3338362329896</v>
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D24" s="64" t="s">
+      <c r="D24" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66">
+      <c r="E24" s="61"/>
+      <c r="F24" s="62">
         <f>F23/(100-E24)*100-F23</f>
         <v>0</v>
       </c>
-      <c r="G24" s="60"/>
-      <c r="H24" s="64" t="s">
+      <c r="G24" s="56"/>
+      <c r="H24" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="65">
+      <c r="I24" s="61">
         <v>20</v>
       </c>
-      <c r="J24" s="66">
+      <c r="J24" s="62">
         <f>J23/(100-I24)*100-J23</f>
         <v>283.01389690721658</v>
       </c>
-      <c r="K24" s="60"/>
-      <c r="L24" s="64" t="s">
+      <c r="K24" s="56"/>
+      <c r="L24" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="65">
+      <c r="M24" s="61">
         <v>10</v>
       </c>
-      <c r="N24" s="66">
+      <c r="N24" s="62">
         <f>N23/(100-M24)*100-N23</f>
         <v>275.03709291477662</v>
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="65"/>
-      <c r="F25" s="66">
+      <c r="E25" s="61"/>
+      <c r="F25" s="62">
         <f>F23+F24</f>
         <v>440.24342400000012</v>
       </c>
-      <c r="G25" s="60"/>
-      <c r="H25" s="64" t="s">
+      <c r="G25" s="56"/>
+      <c r="H25" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="65"/>
-      <c r="J25" s="66">
+      <c r="I25" s="61"/>
+      <c r="J25" s="62">
         <f>J23+J24</f>
         <v>1415.0694845360827</v>
       </c>
-      <c r="K25" s="60"/>
-      <c r="L25" s="64" t="s">
+      <c r="K25" s="56"/>
+      <c r="L25" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="65"/>
-      <c r="N25" s="66">
+      <c r="M25" s="61"/>
+      <c r="N25" s="62">
         <f>N23+N24</f>
         <v>2750.3709291477662</v>
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D26" s="64" t="s">
+      <c r="D26" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="65">
+      <c r="E26" s="61">
         <v>19</v>
       </c>
-      <c r="F26" s="66">
+      <c r="F26" s="62">
         <f>F25/100*E26</f>
         <v>83.646250560000027</v>
       </c>
-      <c r="G26" s="60"/>
-      <c r="H26" s="64" t="s">
+      <c r="G26" s="56"/>
+      <c r="H26" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="65">
+      <c r="I26" s="61">
         <v>19</v>
       </c>
-      <c r="J26" s="66">
+      <c r="J26" s="62">
         <f>J25/100*I26</f>
         <v>268.8632020618557</v>
       </c>
-      <c r="K26" s="60"/>
-      <c r="L26" s="64" t="s">
+      <c r="K26" s="56"/>
+      <c r="L26" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="M26" s="65">
+      <c r="M26" s="61">
         <v>19</v>
       </c>
-      <c r="N26" s="66">
+      <c r="N26" s="62">
         <f>N25/100*M26</f>
         <v>522.57047653807558</v>
       </c>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="66">
+      <c r="E27" s="61"/>
+      <c r="F27" s="62">
         <f>F25+F26</f>
         <v>523.88967456000012</v>
       </c>
-      <c r="G27" s="60"/>
-      <c r="H27" s="64" t="s">
+      <c r="G27" s="56"/>
+      <c r="H27" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="65"/>
-      <c r="J27" s="66">
+      <c r="I27" s="61"/>
+      <c r="J27" s="62">
         <f>J25+J26</f>
         <v>1683.9326865979383</v>
       </c>
-      <c r="K27" s="60"/>
-      <c r="L27" s="64" t="s">
+      <c r="K27" s="56"/>
+      <c r="L27" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="M27" s="65"/>
-      <c r="N27" s="66">
+      <c r="M27" s="61"/>
+      <c r="N27" s="62">
         <f>N25+N26</f>
         <v>3272.9414056858418</v>
       </c>
@@ -3445,8 +3445,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3908,31 +3908,31 @@
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
       <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="18"/>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="58"/>
+      <c r="D2" s="65"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="58"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B3" s="19" t="s">
@@ -3961,7 +3961,7 @@
       <c r="C4" s="16"/>
       <c r="D4" s="21">
         <f>D6+D5</f>
-        <v>130.11778392375751</v>
+        <v>83.510905878421738</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>52</v>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="D5" s="22">
         <f>D6/(1-C5)*C5</f>
-        <v>19.517667588563626</v>
+        <v>12.526635881763262</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>53</v>
@@ -4001,7 +4001,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="22">
         <f>D8+D7</f>
-        <v>110.60011633519389</v>
+        <v>70.984269996658483</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="D7" s="22">
         <f>D8/(1-C7)*C7</f>
-        <v>3.3180034900558164</v>
+        <v>2.1295280998997543</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>12</v>
@@ -4041,7 +4041,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="22">
         <f>D10-D9</f>
-        <v>107.28211284513807</v>
+        <v>68.854741896758725</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>14</v>
@@ -4075,7 +4075,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="23">
         <f>D12-D11</f>
-        <v>115.28211284513807</v>
+        <v>76.854741896758725</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>54</v>
@@ -4090,10 +4090,12 @@
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D11" s="24">
         <f>D12/(1+C11)*C11</f>
-        <v>0</v>
+        <v>38.427370948379355</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>20</v>
@@ -5392,6 +5394,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008A81759B7DFB004A8599E6F327A8EB98" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="16c538c27c9e089401d5678f760f8f49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="57e862f9-3287-4edb-8d69-92d4fb48d952" xmlns:ns3="e3667e19-af09-407c-b0d0-da75c7fe26e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c8fc48563e86c113fea55823a3af8a3" ns2:_="" ns3:_="">
     <xsd:import namespace="57e862f9-3287-4edb-8d69-92d4fb48d952"/>
@@ -5556,22 +5573,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3849BBA7-7FA9-45F9-B49C-CDA374FE0A9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD45D79A-6B5D-420C-8BFA-1B16B2988657}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A7BA2F-D5C3-4BB2-894A-06A0BD77C7DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5588,21 +5607,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD45D79A-6B5D-420C-8BFA-1B16B2988657}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3849BBA7-7FA9-45F9-B49C-CDA374FE0A9A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>